<commit_message>
Calculated new phase Spaces.
</commit_message>
<xml_diff>
--- a/Setup/MazeDimensions_ant.xlsx
+++ b/Setup/MazeDimensions_ant.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>exit_size</t>
   </si>
@@ -156,6 +156,9 @@
   </si>
   <si>
     <t>SL_RASH</t>
+  </si>
+  <si>
+    <t>XL_H arena length used to be 35.2</t>
   </si>
 </sst>
 </file>
@@ -473,15 +476,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -501,7 +504,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -521,7 +524,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -541,7 +544,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -561,7 +564,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -581,12 +584,12 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7">
-        <v>35.200000000000003</v>
+        <v>25</v>
       </c>
       <c r="C7">
         <v>15</v>
@@ -600,8 +603,11 @@
       <c r="F7">
         <v>0.40600000000000003</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="M7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -621,7 +627,7 @@
         <v>0.40600000000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -641,7 +647,7 @@
         <v>0.40600000000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -661,7 +667,7 @@
         <v>0.30449999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -681,7 +687,7 @@
         <v>0.30449999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -701,7 +707,7 @@
         <v>0.30449999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -721,7 +727,7 @@
         <v>0.20300000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>

</xml_diff>